<commit_message>
wrong pin error warning added
</commit_message>
<xml_diff>
--- a/doc/calculator.xlsx
+++ b/doc/calculator.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E205D6-FD44-46BD-8A94-8450AF2A8C08}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5CC14B0-68C7-463E-B20C-B284D789DC47}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="memory calc" sheetId="1" r:id="rId1"/>
+    <sheet name="pins esp8266" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -52,7 +53,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -62,6 +63,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -93,7 +100,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -105,6 +112,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -122,6 +133,109 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1025" name="AutoShape 1" descr="https://microcontrollerslab.com/wp-content/uploads/2019/05/ESP8266-12E-NodeMCU-Development-Board-pinout.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA877D90-ABAF-4B55-A17D-3E01D47D73BE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1219200" y="1645920"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>525781</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>136571</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93082A59-5EE2-42D2-A250-E792F6ADDF9C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2781301" y="304800"/>
+          <a:ext cx="4312919" cy="3489371"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -389,12 +503,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="D4:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="2.44140625" customWidth="1"/>
+    <col min="2" max="2" width="3.77734375" customWidth="1"/>
+    <col min="3" max="3" width="4.44140625" customWidth="1"/>
     <col min="4" max="5" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
@@ -578,4 +695,196 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47D897F4-A422-44DA-97A4-D4FEBA05B735}">
+  <dimension ref="B1:C104"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="7.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="6">
+        <v>0</v>
+      </c>
+      <c r="C3" s="6"/>
+    </row>
+    <row r="4" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="6">
+        <v>1</v>
+      </c>
+      <c r="C4" s="6"/>
+    </row>
+    <row r="5" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="6">
+        <v>2</v>
+      </c>
+      <c r="C5" s="6"/>
+    </row>
+    <row r="6" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="6">
+        <v>3</v>
+      </c>
+      <c r="C6" s="6"/>
+    </row>
+    <row r="7" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="6">
+        <v>4</v>
+      </c>
+      <c r="C7" s="6"/>
+    </row>
+    <row r="8" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="6">
+        <v>5</v>
+      </c>
+      <c r="C8" s="6"/>
+    </row>
+    <row r="9" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="6">
+        <v>9</v>
+      </c>
+      <c r="C9" s="6"/>
+    </row>
+    <row r="10" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="6">
+        <v>10</v>
+      </c>
+      <c r="C10" s="6"/>
+    </row>
+    <row r="11" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="6">
+        <v>12</v>
+      </c>
+      <c r="C11" s="6"/>
+    </row>
+    <row r="12" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="6">
+        <v>13</v>
+      </c>
+      <c r="C12" s="6"/>
+    </row>
+    <row r="13" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="6">
+        <v>14</v>
+      </c>
+      <c r="C13" s="6"/>
+    </row>
+    <row r="14" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="6">
+        <v>15</v>
+      </c>
+      <c r="C14" s="6"/>
+    </row>
+    <row r="15" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="6">
+        <v>16</v>
+      </c>
+      <c r="C15" s="6"/>
+    </row>
+    <row r="16" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="17" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="18" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="19" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="20" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="21" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="22" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="23" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="24" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="25" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="26" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="27" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="28" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="29" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="30" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="31" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="32" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="33" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="34" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="35" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="36" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="37" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="38" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="39" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="40" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="41" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="42" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="43" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="44" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="45" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="46" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="47" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="48" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="49" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="50" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="51" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="52" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="53" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="54" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="55" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="56" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="57" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="58" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="59" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="60" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="61" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="62" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="63" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="64" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="65" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="66" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="67" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="68" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="69" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="70" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="71" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="72" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="73" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="74" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="75" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="76" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="77" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="78" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="79" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="80" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="81" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="82" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="83" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="84" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="85" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="86" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="87" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="88" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="89" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="90" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="91" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="92" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="93" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="94" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="95" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="96" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="97" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="98" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="99" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="100" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="101" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="102" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="103" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="104" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <sortState ref="B3:B15">
+    <sortCondition ref="B3"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>